<commit_message>
update time to game's development lines
</commit_message>
<xml_diff>
--- a/GM_development_process.xlsx
+++ b/GM_development_process.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>镜头</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -105,6 +105,34 @@
   </si>
   <si>
     <t>完成时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习C++和SDL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020/1-2020/2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020/3-2020/6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020/7-2020/12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yu&amp;Xue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -136,15 +164,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -193,23 +239,40 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color theme="4"/>
       </left>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
-        <color theme="4"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -219,7 +282,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color theme="4"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -228,7 +291,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color theme="4"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -239,7 +302,35 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color theme="4"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -251,41 +342,19 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -294,9 +363,11 @@
       <right style="thin">
         <color theme="4"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -304,29 +375,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,36 +750,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A8:P16"/>
+  <dimension ref="A2:P16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="10.75" customWidth="1"/>
-    <col min="6" max="6" width="11.75" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
     <col min="7" max="7" width="22.5" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="8" max="8" width="8.125" customWidth="1"/>
+    <col min="9" max="9" width="7.875" customWidth="1"/>
     <col min="11" max="11" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:16">
+      <c r="B2" s="28"/>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="B3" s="29"/>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="B4" s="27"/>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="4" t="s">
+      <c r="G8" s="15" t="s">
         <v>13</v>
       </c>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="12" t="s">
+      <c r="L8" s="8" t="s">
         <v>18</v>
       </c>
       <c r="M8" s="4" t="s">
@@ -697,168 +806,181 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="5"/>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="13" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="13" t="s">
+      <c r="E9" s="10"/>
+      <c r="F9" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-    </row>
-    <row r="10" spans="1:16" ht="42.75">
+      <c r="G9" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="1:16" ht="57">
       <c r="A10" s="5"/>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="13" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15" t="s">
+      <c r="F10" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="13" t="s">
+      <c r="G10" s="10"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
     </row>
     <row r="11" spans="1:16" ht="28.5">
       <c r="A11" s="5"/>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="13" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15" t="s">
+      <c r="F11" s="10"/>
+      <c r="G11" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="13" t="s">
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="5"/>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="13" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="13" t="s">
+      <c r="G12" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="13" t="s">
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="5"/>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14" t="s">
+      <c r="C13" s="10"/>
+      <c r="D13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
+      <c r="E13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="5"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="7"/>
+      <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="11"/>
+      <c r="K14" s="7"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="19" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="17"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="10"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>